<commit_message>
worked on colab and added saved model
</commit_message>
<xml_diff>
--- a/doc/model_study.xlsx
+++ b/doc/model_study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Google Drive\Drive personal\dev\TinyML\Smart-Alarm-using-tinyML\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0392F1-386D-45B1-86F0-2A9BE676207D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBE5EF0-7CDB-4382-BA14-57F16E80B06C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9A6803E5-358F-4BAD-9F4A-AF61FF455B02}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
   <si>
     <t>Add Movement Features</t>
   </si>
@@ -33,21 +33,12 @@
     <t>No</t>
   </si>
   <si>
-    <t>Otras Features</t>
-  </si>
-  <si>
     <t>Drop Time</t>
   </si>
   <si>
     <t>Heart Rate Normalized</t>
   </si>
   <si>
-    <t>Other features Normalized</t>
-  </si>
-  <si>
-    <t>Nº capas</t>
-  </si>
-  <si>
     <t>3 (64,64,64)</t>
   </si>
   <si>
@@ -57,60 +48,15 @@
     <t>categorical</t>
   </si>
   <si>
-    <t>optimizer</t>
-  </si>
-  <si>
     <t>adam</t>
   </si>
   <si>
-    <t>epochs</t>
-  </si>
-  <si>
-    <t>Resultados</t>
-  </si>
-  <si>
-    <t>train</t>
-  </si>
-  <si>
-    <t>validation</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>loss train</t>
-  </si>
-  <si>
-    <t>loss validation</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Tiempo </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>entrenamiento</t>
-    </r>
-  </si>
-  <si>
-    <t>overfitting</t>
-  </si>
-  <si>
     <t>513s</t>
   </si>
   <si>
     <t>no</t>
   </si>
   <si>
-    <t>loss test</t>
-  </si>
-  <si>
     <t>463s</t>
   </si>
   <si>
@@ -120,9 +66,6 @@
     <t>473s</t>
   </si>
   <si>
-    <t>Autofeat genera Features</t>
-  </si>
-  <si>
     <t>Test 1</t>
   </si>
   <si>
@@ -138,19 +81,70 @@
     <t>Test 5</t>
   </si>
   <si>
-    <t>Balanced labels</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>Yes (x3,y3,z3)</t>
   </si>
   <si>
-    <t>batch Yesze</t>
-  </si>
-  <si>
-    <t>ConfuYeson matrix</t>
+    <t>Autofeat generated Features</t>
+  </si>
+  <si>
+    <t>Other Features</t>
+  </si>
+  <si>
+    <t>Other feautres Normalized</t>
+  </si>
+  <si>
+    <t>Number of layers</t>
+  </si>
+  <si>
+    <t>Optimizer</t>
+  </si>
+  <si>
+    <t>Epochs</t>
+  </si>
+  <si>
+    <t>Batch size</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Training time</t>
+  </si>
+  <si>
+    <t>It overfitted</t>
+  </si>
+  <si>
+    <t>Accuracy training</t>
+  </si>
+  <si>
+    <t>Loss training</t>
+  </si>
+  <si>
+    <t>Accuracy validation</t>
+  </si>
+  <si>
+    <t>Loss validation</t>
+  </si>
+  <si>
+    <t>Accuracy test</t>
+  </si>
+  <si>
+    <t>Loss Test</t>
+  </si>
+  <si>
+    <t>Confussion Matrix</t>
+  </si>
+  <si>
+    <t>Test 6</t>
+  </si>
+  <si>
+    <t>Balanced dataset (undersampled labels)</t>
+  </si>
+  <si>
+    <t>Yes (**2, **3, exp)</t>
   </si>
 </sst>
 </file>
@@ -862,80 +856,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155B3322-AD04-40C2-981B-3E80C2F0D10D}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="1"/>
     <col min="3" max="3" width="11.42578125" style="12"/>
     <col min="4" max="4" width="11.42578125" style="20"/>
     <col min="5" max="6" width="12.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="17" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -943,21 +947,24 @@
         <v>1</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -974,10 +981,13 @@
       <c r="F5" s="12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -989,115 +999,124 @@
         <v>1</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="C9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F11" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1">
         <v>150</v>
@@ -1115,9 +1134,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1">
         <v>180</v>
@@ -1135,48 +1154,48 @@
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B18" s="10">
         <v>0.39</v>
@@ -1194,7 +1213,7 @@
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B19" s="4">
         <v>1.3821000000000001</v>
@@ -1212,7 +1231,7 @@
     </row>
     <row r="20" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B20" s="10">
         <v>0.42</v>
@@ -1230,7 +1249,7 @@
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B21" s="4">
         <v>1.3524</v>
@@ -1248,7 +1267,7 @@
     </row>
     <row r="22" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B22" s="10">
         <v>0.41</v>
@@ -1266,7 +1285,7 @@
     </row>
     <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B23" s="4">
         <v>1.3543959999999999</v>
@@ -1284,7 +1303,7 @@
     </row>
     <row r="24" spans="1:6" s="3" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24"/>
       <c r="C24" s="12"/>

</xml_diff>